<commit_message>
Added Apple.txt, Banana.txt, Cream.txt | Modified Book1.xlsx, Cheat_Sheet.txt, Resume.docx, test1.txt
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Candidates Details</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>Postman</t>
+  </si>
+  <si>
+    <t>Balu</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -66,10 +78,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -94,17 +106,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,6 +129,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -135,22 +154,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -164,6 +168,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -173,12 +185,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -189,29 +215,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,6 +245,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -240,180 +426,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,6 +448,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -451,17 +478,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -469,8 +490,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,71 +536,62 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -589,88 +601,88 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1003,13 +1015,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3"/>
   <cols>
     <col min="3" max="3" width="12.3333333333333" customWidth="1"/>
     <col min="4" max="4" width="14.1111111111111" customWidth="1"/>
@@ -1090,6 +1102,32 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>